<commit_message>
Improved layout with bootstrap classes.
</commit_message>
<xml_diff>
--- a/data/EPFL Extension School-Personal Details-MASTER-for Daniel-02SEP2020.xlsx
+++ b/data/EPFL Extension School-Personal Details-MASTER-for Daniel-02SEP2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dflores/Dropbox/EXTS/Projects/autoHiring/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dflores/Google Drive/EXTS/Projects/autoHiring/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A52167-3950-E440-AEB3-81EA268EEAAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF75151-D41D-EA48-B18A-5BF1B8A7093A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{7A64A84C-17F9-2548-864F-7F5C3007427B}"/>
+    <workbookView xWindow="26380" yWindow="460" windowWidth="24820" windowHeight="28340" activeTab="2" xr2:uid="{7A64A84C-17F9-2548-864F-7F5C3007427B}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="111">
   <si>
     <t>First Name</t>
   </si>
@@ -329,9 +329,6 @@
     <t>CDT?</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>AVS card?</t>
   </si>
   <si>
@@ -354,12 +351,6 @@
   </si>
   <si>
     <t>Nico Schuele</t>
-  </si>
-  <si>
-    <t>SMITH</t>
-  </si>
-  <si>
-    <t>Francesca</t>
   </si>
   <si>
     <t>Intro CdC string</t>
@@ -504,14 +495,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -543,9 +531,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -888,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D2E135-155D-3F42-BE22-6B196658E3B7}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,12 +884,12 @@
     <col min="3" max="3" width="23" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:3" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -915,7 +900,7 @@
       <c r="B4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="23" t="s">
         <v>60</v>
       </c>
     </row>
@@ -923,280 +908,330 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <v>30992</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="16">
+        <v>30992</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="14" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="16">
         <v>38852</v>
       </c>
-      <c r="C19" s="18"/>
+      <c r="C19" s="16">
+        <v>38852</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="14" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="14" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="16">
         <v>44105</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="16">
+        <v>44105</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="18"/>
+      <c r="C26" s="24" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="24" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="18"/>
+        <v>101</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>100</v>
+      <c r="C30" s="24" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>89</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="18"/>
+      <c r="C31" s="24" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="15">
         <v>0.8</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="15">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1213,179 +1248,179 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.1640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="121.5" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="53.1640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="121.5" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:3" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="10" t="str">
+      <c r="B3" s="9" t="str">
         <f>Details!C5</f>
-        <v>SMITH</v>
-      </c>
-      <c r="C3" s="7"/>
+        <v>MOSER</v>
+      </c>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="10" t="str">
+      <c r="B4" s="9" t="str">
         <f>Details!C6</f>
-        <v>Francesca</v>
-      </c>
-      <c r="C4" s="7"/>
+        <v>Laure</v>
+      </c>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>Details!C8</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="7"/>
+        <v>30992</v>
+      </c>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9" t="str">
         <f>Details!C20</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="7"/>
+        <v>Business Administration</v>
+      </c>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <f>Details!C25</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="7"/>
+        <v>44105</v>
+      </c>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9" t="str">
         <f>Details!C32</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="7"/>
+        <v>Course Developer and Instructor</v>
+      </c>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <f>Details!C25</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="7"/>
+        <v>44105</v>
+      </c>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="14" t="str">
+      <c r="A14" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="13" t="str">
         <f>_xlfn.CONCAT(Details!C6," ",Details!C5," is hired as a ",Details!B32," for the ",Details!B33," team of the EPFL Extension School, under the supervision of  ",CdC!B19,". S/he will focus on the following key tasks:")</f>
-        <v>Francesca SMITH is hired as a Course Developer and Instructor for the Web/Code team of the EPFL Extension School, under the supervision of  Nico Schuele. S/he will focus on the following key tasks:</v>
-      </c>
-      <c r="C14" s="7"/>
+        <v>Laure MOSER is hired as a Course Developer and Instructor for the Web/Code team of the EPFL Extension School, under the supervision of  Nico Schuele. S/he will focus on the following key tasks:</v>
+      </c>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" ht="291" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="B18" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="7"/>
+      <c r="C19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1396,125 +1431,125 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A10DC8F1-3DAA-4E40-8C8C-49D0E157B43C}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="29.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" style="7" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="24" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:2" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
+      <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="17">
         <f>Details!C25</f>
-        <v>0</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <f>DATE(YEAR(B4) + 1, MONTH(B4), DAY(B4))</f>
-        <v>366</v>
+        <v>44470</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>11262</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="10" t="str">
+      <c r="B10" s="9" t="str">
         <f>Details!C5</f>
-        <v>SMITH</v>
+        <v>MOSER</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="10" t="str">
+      <c r="B11" s="9" t="str">
         <f>Details!C6</f>
-        <v>Francesca</v>
+        <v>Laure</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9" t="str">
         <f>Details!C7</f>
-        <v>0</v>
+        <v>756.33.3412.3234</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9" t="str">
         <f>Details!C9</f>
-        <v>0</v>
+        <v>route de France</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <f>Details!C10</f>
         <v>0</v>
       </c>
@@ -1523,198 +1558,198 @@
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9" t="str">
         <f>Details!C11</f>
-        <v>0</v>
+        <v>Lausanne</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9" t="str">
         <f>Details!C12</f>
-        <v>0</v>
+        <v>VD</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="9" t="str">
         <f>Details!C13</f>
-        <v>0</v>
+        <v>Switzerland</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="17">
         <f>Details!C8</f>
-        <v>0</v>
+        <v>30992</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9" t="str">
         <f>Details!C14</f>
-        <v>0</v>
+        <v>Married</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <f>Details!C15</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9" t="str">
         <f>Details!C22</f>
-        <v>0</v>
+        <v>GE</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9" t="str">
         <f>Details!C21</f>
-        <v>0</v>
+        <v>Swiss</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="9" t="str">
         <f>Details!C20</f>
-        <v>0</v>
+        <v>Business Administration</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="9" t="str">
         <f>Details!C16</f>
-        <v>0</v>
+        <v>No</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="17">
         <f>Details!C19</f>
-        <v>0</v>
+        <v>38852</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="17" t="str">
         <f>Details!C17</f>
-        <v>0</v>
+        <v>--</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="18">
         <f>Details!C34</f>
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="19" t="str">
         <f>Details!C35</f>
-        <v>0</v>
+        <v>Lausanne / Geneva</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="9" t="str">
         <f>Details!C24</f>
-        <v>0</v>
+        <v>--</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="7" t="str">
+      <c r="B30" s="6" t="e">
         <f>IF(Details!C26&lt;&gt;"",YES,"")</f>
-        <v/>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="7" t="str">
+      <c r="B31" s="6" t="str">
         <f>IF(Details!C27&lt;&gt;"","YES","")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="7" t="str">
+      <c r="B32" s="6" t="str">
         <f>IF(Details!C28&lt;&gt;"","YES","")</f>
-        <v/>
+        <v>YES</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="7" t="str">
+      <c r="A33" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="6" t="str">
         <f>IF(Details!C29&lt;&gt;"","YES","")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="7" t="str">
+      <c r="B34" s="6" t="str">
         <f>IF(Details!C30&lt;&gt;"","YES","")</f>
         <v>YES</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="7" t="str">
+      <c r="B35" s="6" t="str">
         <f>IF(Details!C31&lt;&gt;"","YES","")</f>
-        <v/>
+        <v>YES</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="7" t="str">
+      <c r="B36" s="6" t="str">
         <f>IF(Details!C32&lt;&gt;"","YES","")</f>
-        <v/>
+        <v>YES</v>
       </c>
     </row>
   </sheetData>

</xml_diff>